<commit_message>
Matplotlib agg para plotar, necessário colocar plt.show() no arquivo plots.py
</commit_message>
<xml_diff>
--- a/data/results/df_daily_return_ppo.xlsx
+++ b/data/results/df_daily_return_ppo.xlsx
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0230067256535316</v>
+        <v>0.02051435734447838</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0019102974811915</v>
+        <v>-0.0001375096831625344</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.002657538712712603</v>
+        <v>8.305288303231905e-05</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.02188027661298455</v>
+        <v>0.02579723778711187</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.006017562776586828</v>
+        <v>-0.005825733028860881</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.005346428884788928</v>
+        <v>0.005833829896371486</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.001138419996192675</v>
+        <v>0.001062550162739401</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.005659767829942442</v>
+        <v>-0.002332471335930176</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.001424517855894126</v>
+        <v>-0.003576702922601704</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.001595412715376184</v>
+        <v>0.003106258467134456</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01956057026765519</v>
+        <v>0.01984543428669502</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.002958005104533843</v>
+        <v>0.003023307893114284</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.01421528180737992</v>
+        <v>0.01938765214175742</v>
       </c>
     </row>
     <row r="16">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.004413910265712231</v>
+        <v>-0.002660651770497854</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.003294985431378664</v>
+        <v>0.002590669954575491</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.02201816068487972</v>
+        <v>-0.0234845557800854</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.03835497044203626</v>
+        <v>-0.03509710545456971</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.006671034164699706</v>
+        <v>0.009562527717395372</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.02038551948606907</v>
+        <v>-0.02349751251101369</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.01959832693773523</v>
+        <v>0.02162647400210408</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.01226476410478835</v>
+        <v>0.00937492454114998</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.02045433716595819</v>
+        <v>0.01968607346541905</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.002694238617054173</v>
+        <v>-0.004563834505195126</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.01852926154207173</v>
+        <v>0.03273956033000804</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.02777061958560266</v>
+        <v>0.03130790025388665</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.006742921898078147</v>
+        <v>-0.006714583845418093</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.02209602670613867</v>
+        <v>-0.02197151076693475</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.02302515793984682</v>
+        <v>0.02041100812541597</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01845390795606485</v>
+        <v>0.0168547971460298</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.004395890075366515</v>
+        <v>0.005076559319618838</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.008068648968217698</v>
+        <v>-0.01143158872470887</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.001187092223832816</v>
+        <v>0.000223076087560152</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.0005282218957526402</v>
+        <v>0.00304450553521832</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.02389149519207168</v>
+        <v>0.02390376518836063</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.003534681300226507</v>
+        <v>-0.003251529956255575</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.002203381642667785</v>
+        <v>0.003936250235822492</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.007183543916663145</v>
+        <v>0.00562469631379969</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>-0.0125507217017198</v>
+        <v>-0.01473252992039143</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.03028091585852476</v>
+        <v>0.02850867434981026</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.001016457981436184</v>
+        <v>0.006143394398916415</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>-0.007256918029079539</v>
+        <v>-0.003455378746039343</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.01449327461604566</v>
+        <v>0.01430316425622114</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>-0.003909620684731543</v>
+        <v>-0.001512551533702053</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.003262957503418667</v>
+        <v>0.001734896453142683</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.001145007979578776</v>
+        <v>0.002394796986218513</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.02496224253010335</v>
+        <v>0.02596154307477862</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.006883201116348645</v>
+        <v>0.01054674349189588</v>
       </c>
     </row>
     <row r="50">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>-0.007083514674893522</v>
+        <v>-0.006902313585903123</v>
       </c>
     </row>
     <row r="51">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.01401422828004202</v>
+        <v>0.01074859235451519</v>
       </c>
     </row>
     <row r="52">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.01303238644683718</v>
+        <v>0.01468183974347432</v>
       </c>
     </row>
     <row r="53">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.001402340882088126</v>
+        <v>0.003302991955857197</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.00119679144785103</v>
+        <v>0.001076453461456259</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>-0.02240979299802723</v>
+        <v>-0.02072208113356628</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.008527056438927446</v>
+        <v>0.01110123930485388</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.004279483166820078</v>
+        <v>0.003729709518888322</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.01137647000463846</v>
+        <v>0.01062753540114113</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.005368409631197704</v>
+        <v>0.00462609702168591</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.004560773708910596</v>
+        <v>0.000702327383818287</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>-0.005422045787823833</v>
+        <v>-0.007064380390388275</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.001247309196186646</v>
+        <v>0.0007140330785131938</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.007806976563863885</v>
+        <v>0.01036101706502311</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.02951609359932767</v>
+        <v>0.03509093659862879</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.01725529009870125</v>
+        <v>0.01534233037558532</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>-0.02137252249679726</v>
+        <v>-0.01707234452328786</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>-0.01714416057790908</v>
+        <v>-0.008482911060907056</v>
       </c>
     </row>
     <row r="68">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.01124711667559102</v>
+        <v>0.007543263013162283</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>-0.021820781638366</v>
+        <v>-0.02119585294863701</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.00396486316358914</v>
+        <v>0.003720045829255648</v>
       </c>
     </row>
     <row r="71">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-0.001947403033541027</v>
+        <v>-0.002297676235293499</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>-0.009163622988324001</v>
+        <v>-0.009945297379298963</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>-0.0144122226456236</v>
+        <v>-0.01154810866095678</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>-0.01527028640151858</v>
+        <v>-0.01311149138160481</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>-0.008978843661881676</v>
+        <v>-0.01042533578900092</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>-0.002009525317405508</v>
+        <v>-0.002715381752200662</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.02199412831527444</v>
+        <v>0.0244933068019604</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>-0.02337547049696435</v>
+        <v>-0.02483406411740836</v>
       </c>
     </row>
     <row r="79">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.02806131606938136</v>
+        <v>0.03319973157667867</v>
       </c>
     </row>
     <row r="80">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>-0.0009360040368446684</v>
+        <v>0.002697138856993156</v>
       </c>
     </row>
     <row r="81">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.013077062174906</v>
+        <v>0.01400880246388621</v>
       </c>
     </row>
     <row r="82">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-0.0006777830981333131</v>
+        <v>-0.002874348434137302</v>
       </c>
     </row>
     <row r="83">
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.00589867625407588</v>
+        <v>0.007324260532039726</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>-0.01239517359216263</v>
+        <v>-0.01215943203034563</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>-0.0007567645298500974</v>
+        <v>-0.002421900685187426</v>
       </c>
     </row>
     <row r="86">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.002747750202881488</v>
+        <v>-0.003628164412089449</v>
       </c>
     </row>
     <row r="87">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.005956821807763679</v>
+        <v>0.005691173313013595</v>
       </c>
     </row>
     <row r="88">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>-0.001784080506787157</v>
+        <v>0.00596927349170409</v>
       </c>
     </row>
     <row r="89">
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>-0.003731298810012617</v>
+        <v>-0.008087148964457953</v>
       </c>
     </row>
     <row r="90">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>-0.05455354849972833</v>
+        <v>-0.04012147107749704</v>
       </c>
     </row>
     <row r="91">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.03592126693318064</v>
+        <v>0.02840371658338257</v>
       </c>
     </row>
     <row r="92">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.0005113604016564015</v>
+        <v>0.004112370370237574</v>
       </c>
     </row>
     <row r="93">
@@ -1638,7 +1638,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>-0.02601377279783528</v>
+        <v>-0.02763824681084825</v>
       </c>
     </row>
     <row r="94">
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>-0.02108785481081334</v>
+        <v>-0.02607174950369251</v>
       </c>
     </row>
     <row r="95">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>-0.008327041563840988</v>
+        <v>-0.007797282794926744</v>
       </c>
     </row>
     <row r="96">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.01362771125046896</v>
+        <v>0.01471953368257418</v>
       </c>
     </row>
     <row r="97">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>-0.0003065534976447086</v>
+        <v>-0.001474980147440118</v>
       </c>
     </row>
     <row r="98">
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.01693613499906269</v>
+        <v>0.01559001060992371</v>
       </c>
     </row>
     <row r="99">
@@ -1716,7 +1716,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.02653826044004055</v>
+        <v>0.02569882639031697</v>
       </c>
     </row>
     <row r="100">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>-0.03325240902815953</v>
+        <v>-0.03091127204215155</v>
       </c>
     </row>
     <row r="101">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.01358448476596939</v>
+        <v>0.006646597485941096</v>
       </c>
     </row>
     <row r="102">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.002985497516308368</v>
+        <v>0.0005699146127152468</v>
       </c>
     </row>
     <row r="103">
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.007922151418059319</v>
+        <v>0.006742942533548534</v>
       </c>
     </row>
     <row r="104">
@@ -1781,7 +1781,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.005460354221316971</v>
+        <v>0.001954806305100986</v>
       </c>
     </row>
     <row r="105">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>-0.0007901581570104294</v>
+        <v>-0.0039505552793445</v>
       </c>
     </row>
     <row r="106">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.02799973318031606</v>
+        <v>0.02467569038113664</v>
       </c>
     </row>
     <row r="107">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>-0.006332143600847806</v>
+        <v>-2.882217516871977e-09</v>
       </c>
     </row>
     <row r="108">
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.01644541580022337</v>
+        <v>0.006015641209137247</v>
       </c>
     </row>
     <row r="109">
@@ -1846,7 +1846,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>-0.008822254195091445</v>
+        <v>-0.006722776516889137</v>
       </c>
     </row>
     <row r="110">
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>-0.01276643083075498</v>
+        <v>-0.01799979337725179</v>
       </c>
     </row>
     <row r="111">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>-0.00885128044339493</v>
+        <v>-0.003963768538029548</v>
       </c>
     </row>
     <row r="112">
@@ -1885,7 +1885,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.004985498045899211</v>
+        <v>0.008903434169700047</v>
       </c>
     </row>
     <row r="113">
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0.002815772979725299</v>
+        <v>0.005847704722471756</v>
       </c>
     </row>
     <row r="114">
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0.0003243661376231148</v>
+        <v>0.003426285765308</v>
       </c>
     </row>
     <row r="115">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0.005520557682283975</v>
+        <v>0.006332856739910029</v>
       </c>
     </row>
     <row r="116">
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>-0.01300736089217255</v>
+        <v>-0.0125420167111633</v>
       </c>
     </row>
     <row r="117">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>-0.01282624607225797</v>
+        <v>-0.01179917410818732</v>
       </c>
     </row>
     <row r="118">
@@ -1963,7 +1963,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.01460764239317443</v>
+        <v>0.01643064835245211</v>
       </c>
     </row>
     <row r="119">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.004239508618610908</v>
+        <v>0.003525043946617817</v>
       </c>
     </row>
     <row r="120">
@@ -1989,7 +1989,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>-0.001424115398257906</v>
+        <v>-0.002078726052475914</v>
       </c>
     </row>
     <row r="121">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>0.0005892252781108952</v>
+        <v>0.002164242777852014</v>
       </c>
     </row>
     <row r="122">
@@ -2015,7 +2015,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>-0.002308854450283067</v>
+        <v>-0.002859765380563018</v>
       </c>
     </row>
     <row r="123">
@@ -2028,7 +2028,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0.007761016330000613</v>
+        <v>0.004322631166222414</v>
       </c>
     </row>
     <row r="124">
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>-0.0005296527167622236</v>
+        <v>0.005303860478761781</v>
       </c>
     </row>
     <row r="125">
@@ -2054,7 +2054,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>-0.001350464565736085</v>
+        <v>-0.0001956274324654864</v>
       </c>
     </row>
     <row r="126">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.005794313837688808</v>
+        <v>0.007696609866311753</v>
       </c>
     </row>
     <row r="127">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.002206470528257741</v>
+        <v>-0.0007573142225246489</v>
       </c>
     </row>
     <row r="128">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>-0.003665796044498368</v>
+        <v>-0.001560109965805489</v>
       </c>
     </row>
     <row r="129">
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>-0.005629232118197992</v>
+        <v>-0.01022275002372063</v>
       </c>
     </row>
     <row r="130">
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.00967677435444856</v>
+        <v>0.008583934823638575</v>
       </c>
     </row>
     <row r="131">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>-0.002237172365436219</v>
+        <v>-0.0001824346804232672</v>
       </c>
     </row>
     <row r="132">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>-0.01179749535665911</v>
+        <v>-0.008253877124021522</v>
       </c>
     </row>
     <row r="133">
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.02197687376260654</v>
+        <v>0.01370940638795208</v>
       </c>
     </row>
     <row r="134">
@@ -2171,7 +2171,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>-0.005865569503629479</v>
+        <v>-0.01087496546452281</v>
       </c>
     </row>
     <row r="135">
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>-0.005912495361332493</v>
+        <v>-0.00670681117881388</v>
       </c>
     </row>
     <row r="136">
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0.003962504453719748</v>
+        <v>0.0003534827281194825</v>
       </c>
     </row>
     <row r="137">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>-0.01791631349116209</v>
+        <v>-0.01561519106763043</v>
       </c>
     </row>
     <row r="138">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0.01350948081577677</v>
+        <v>0.01238964605658738</v>
       </c>
     </row>
     <row r="139">
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.01498433021811589</v>
+        <v>0.01744952423345932</v>
       </c>
     </row>
     <row r="140">
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.01190681722084721</v>
+        <v>0.01752793642547214</v>
       </c>
     </row>
     <row r="141">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.00652541181146027</v>
+        <v>0.006835324500154278</v>
       </c>
     </row>
     <row r="142">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.01602167042008184</v>
+        <v>0.01278594182128768</v>
       </c>
     </row>
     <row r="143">
@@ -2288,7 +2288,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>-0.01506357747501812</v>
+        <v>-0.01427568334127211</v>
       </c>
     </row>
     <row r="144">
@@ -2301,7 +2301,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0.00655423445440027</v>
+        <v>0.003651490887585052</v>
       </c>
     </row>
     <row r="145">
@@ -2314,7 +2314,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>0.004222996280384123</v>
+        <v>0.005677704740940499</v>
       </c>
     </row>
     <row r="146">
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0.0004471639943607381</v>
+        <v>-0.003000005836666262</v>
       </c>
     </row>
     <row r="147">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0.002123133048248023</v>
+        <v>0.004065849617040903</v>
       </c>
     </row>
     <row r="148">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>-0.006451492896056505</v>
+        <v>-0.006375744118700048</v>
       </c>
     </row>
     <row r="149">
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0.003147570523747729</v>
+        <v>0.002622863141209583</v>
       </c>
     </row>
     <row r="150">
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0.006436176231615727</v>
+        <v>0.004908013828907936</v>
       </c>
     </row>
     <row r="151">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>-0.006473564480278123</v>
+        <v>-0.004629905320527777</v>
       </c>
     </row>
     <row r="152">
@@ -2405,7 +2405,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.006626176422893525</v>
+        <v>0.0006404891491440541</v>
       </c>
     </row>
     <row r="153">
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0.00888114899839702</v>
+        <v>0.007967088109164751</v>
       </c>
     </row>
     <row r="154">
@@ -2431,7 +2431,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0.01150570714792338</v>
+        <v>0.01181414693332584</v>
       </c>
     </row>
     <row r="155">
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.0003242257639286411</v>
+        <v>0.003825242124547813</v>
       </c>
     </row>
     <row r="156">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.01205298546966656</v>
+        <v>0.01011541755906155</v>
       </c>
     </row>
     <row r="157">
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0.009689046587915891</v>
+        <v>0.01365382847329401</v>
       </c>
     </row>
     <row r="158">
@@ -2483,7 +2483,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0.002633175153108435</v>
+        <v>0.003012637547863795</v>
       </c>
     </row>
     <row r="159">
@@ -2496,7 +2496,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0.01221742575106495</v>
+        <v>0.009378398246148414</v>
       </c>
     </row>
     <row r="160">
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>-0.01394408297326621</v>
+        <v>-0.01247314440124957</v>
       </c>
     </row>
     <row r="161">
@@ -2522,7 +2522,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.005496851969869545</v>
+        <v>0.00653557361899672</v>
       </c>
     </row>
     <row r="162">
@@ -2535,7 +2535,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0.002559074162570289</v>
+        <v>-0.003006329698577769</v>
       </c>
     </row>
     <row r="163">
@@ -2548,7 +2548,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>-0.001886311309977795</v>
+        <v>-0.003435693108366187</v>
       </c>
     </row>
     <row r="164">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.0008820033285764791</v>
+        <v>0.001852228325471234</v>
       </c>
     </row>
     <row r="165">
@@ -2574,7 +2574,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>0.00307901862260771</v>
+        <v>-0.00162286970867853</v>
       </c>
     </row>
     <row r="166">
@@ -2587,7 +2587,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0.004562379156826675</v>
+        <v>0.002493088547234747</v>
       </c>
     </row>
     <row r="167">
@@ -2600,7 +2600,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-0.01351815484322783</v>
+        <v>-0.009718040162592183</v>
       </c>
     </row>
     <row r="168">
@@ -2613,7 +2613,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0.006983613686442436</v>
+        <v>0.005030412385775558</v>
       </c>
     </row>
     <row r="169">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0.004106621522790873</v>
+        <v>0.004407655294694672</v>
       </c>
     </row>
     <row r="170">
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-0.008423248848156505</v>
+        <v>-0.0056761141820567</v>
       </c>
     </row>
     <row r="171">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-0.007692166862301272</v>
+        <v>-0.006064460760590201</v>
       </c>
     </row>
     <row r="172">
@@ -2665,7 +2665,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.005923587224498552</v>
+        <v>0.005978634671996524</v>
       </c>
     </row>
     <row r="173">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-0.02374792195015439</v>
+        <v>-0.02571027288664712</v>
       </c>
     </row>
     <row r="174">
@@ -2691,7 +2691,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.005980798901975919</v>
+        <v>0.007106320428541879</v>
       </c>
     </row>
     <row r="175">
@@ -2704,7 +2704,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-0.002901148088856305</v>
+        <v>-0.002320187228931714</v>
       </c>
     </row>
     <row r="176">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-0.007821805768438718</v>
+        <v>-0.006900590831603003</v>
       </c>
     </row>
     <row r="177">
@@ -2730,7 +2730,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-0.006162560740993195</v>
+        <v>-0.004480738624410435</v>
       </c>
     </row>
     <row r="178">
@@ -2743,7 +2743,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0.006408395768927498</v>
+        <v>0.007178835180708563</v>
       </c>
     </row>
     <row r="179">
@@ -2756,7 +2756,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-0.003169698030212604</v>
+        <v>-0.007185451704328711</v>
       </c>
     </row>
     <row r="180">
@@ -2769,7 +2769,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-0.01274172989606947</v>
+        <v>-0.01316678247773962</v>
       </c>
     </row>
     <row r="181">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0.01371164005122227</v>
+        <v>0.01240361774214449</v>
       </c>
     </row>
     <row r="182">
@@ -2795,7 +2795,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-0.01755867829426457</v>
+        <v>-0.01498133765061826</v>
       </c>
     </row>
     <row r="183">
@@ -2808,7 +2808,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0.02104746064229976</v>
+        <v>0.02140856308580248</v>
       </c>
     </row>
     <row r="184">
@@ -2821,7 +2821,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.0002791847885607049</v>
+        <v>0.001694308919124908</v>
       </c>
     </row>
     <row r="185">
@@ -2834,7 +2834,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-0.01396528438173037</v>
+        <v>-0.01514691091542449</v>
       </c>
     </row>
     <row r="186">
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-0.01269913758658708</v>
+        <v>-0.01292098258228662</v>
       </c>
     </row>
     <row r="187">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-0.01274660379115258</v>
+        <v>-0.01496097660195592</v>
       </c>
     </row>
     <row r="188">
@@ -2873,7 +2873,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.008527050219109039</v>
+        <v>0.009342703823630286</v>
       </c>
     </row>
     <row r="189">
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.00274274911631212</v>
+        <v>0.002548247118438769</v>
       </c>
     </row>
     <row r="190">
@@ -2899,7 +2899,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-0.003713119016488041</v>
+        <v>-0.002894834490577225</v>
       </c>
     </row>
     <row r="191">
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-0.006808745514582277</v>
+        <v>-0.007638100821650799</v>
       </c>
     </row>
     <row r="192">
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0.01295383762947403</v>
+        <v>0.01176889138947857</v>
       </c>
     </row>
     <row r="193">
@@ -2938,7 +2938,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-0.007829078193740778</v>
+        <v>-0.007186315420856699</v>
       </c>
     </row>
     <row r="194">
@@ -2951,7 +2951,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0.01217921209699482</v>
+        <v>0.01288280046012008</v>
       </c>
     </row>
     <row r="195">
@@ -2964,7 +2964,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-0.006974354305556413</v>
+        <v>-0.005986875313075053</v>
       </c>
     </row>
     <row r="196">
@@ -2977,7 +2977,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-0.02461254549606674</v>
+        <v>-0.02953262219820569</v>
       </c>
     </row>
     <row r="197">
@@ -2990,7 +2990,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0.009051101845247754</v>
+        <v>0.004069016850059181</v>
       </c>
     </row>
     <row r="198">
@@ -3003,7 +3003,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.006621756260588896</v>
+        <v>0.01082593032328428</v>
       </c>
     </row>
     <row r="199">
@@ -3016,7 +3016,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-0.01262123363078098</v>
+        <v>-0.01376939399164872</v>
       </c>
     </row>
     <row r="200">
@@ -3029,7 +3029,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>0.0002525790138062612</v>
+        <v>-0.006151339332553268</v>
       </c>
     </row>
     <row r="201">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0.01593415329281738</v>
+        <v>0.01452562201090075</v>
       </c>
     </row>
     <row r="202">
@@ -3055,7 +3055,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0.002004854522890947</v>
+        <v>0.004902303994855401</v>
       </c>
     </row>
     <row r="203">
@@ -3068,7 +3068,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-0.01094231480046285</v>
+        <v>-0.01234429926445696</v>
       </c>
     </row>
     <row r="204">
@@ -3081,7 +3081,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-0.002266213154106075</v>
+        <v>-0.0042882937356993</v>
       </c>
     </row>
     <row r="205">
@@ -3094,7 +3094,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-0.003272026950736583</v>
+        <v>0.00033787893669382</v>
       </c>
     </row>
     <row r="206">
@@ -3107,7 +3107,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-0.01076751194176094</v>
+        <v>-0.01235769970659253</v>
       </c>
     </row>
     <row r="207">
@@ -3120,7 +3120,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-0.004889371515570872</v>
+        <v>-0.005493907563614209</v>
       </c>
     </row>
     <row r="208">
@@ -3133,7 +3133,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-0.007102277940664753</v>
+        <v>-0.01470581312505657</v>
       </c>
     </row>
     <row r="209">
@@ -3146,7 +3146,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.003174375661755849</v>
+        <v>0.007271154461730368</v>
       </c>
     </row>
     <row r="210">
@@ -3159,7 +3159,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.008212496697555086</v>
+        <v>0.01335994738926758</v>
       </c>
     </row>
     <row r="211">
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>0.001911878091327444</v>
+        <v>-0.005376969424788742</v>
       </c>
     </row>
     <row r="212">
@@ -3185,7 +3185,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>0.02413317633528658</v>
+        <v>0.02217491077780689</v>
       </c>
     </row>
     <row r="213">
@@ -3198,7 +3198,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>0.005357372214287648</v>
+        <v>0.01018052397502896</v>
       </c>
     </row>
     <row r="214">
@@ -3211,7 +3211,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-0.01612537732271267</v>
+        <v>-0.01623462358525367</v>
       </c>
     </row>
     <row r="215">
@@ -3224,7 +3224,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>0.01206362139801017</v>
+        <v>0.01295285609619496</v>
       </c>
     </row>
     <row r="216">
@@ -3237,7 +3237,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-0.006185065439169458</v>
+        <v>-0.006047928473536031</v>
       </c>
     </row>
     <row r="217">
@@ -3250,7 +3250,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>-0.0009331770176965945</v>
+        <v>-0.005525642887297968</v>
       </c>
     </row>
     <row r="218">
@@ -3263,7 +3263,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.0005556295169479948</v>
+        <v>0.002625363006218896</v>
       </c>
     </row>
     <row r="219">
@@ -3276,7 +3276,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>-0.02666375927851342</v>
+        <v>-0.02835702969737758</v>
       </c>
     </row>
     <row r="220">
@@ -3289,7 +3289,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>-0.0003241981143093702</v>
+        <v>0.001021872997220459</v>
       </c>
     </row>
     <row r="221">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>0.01112492732208694</v>
+        <v>0.01225389782688378</v>
       </c>
     </row>
     <row r="222">
@@ -3315,7 +3315,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>-0.04159020867275746</v>
+        <v>-0.04577073285731705</v>
       </c>
     </row>
     <row r="223">
@@ -3328,7 +3328,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>0.01555140738937464</v>
+        <v>0.02066984771095196</v>
       </c>
     </row>
     <row r="224">
@@ -3341,7 +3341,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>-0.005659725199164719</v>
+        <v>-0.009540201683117264</v>
       </c>
     </row>
     <row r="225">
@@ -3354,7 +3354,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>0.01654782317731995</v>
+        <v>0.01828071343772742</v>
       </c>
     </row>
     <row r="226">
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>-0.0002382074045954587</v>
+        <v>-0.0005503458119990293</v>
       </c>
     </row>
     <row r="227">
@@ -3380,7 +3380,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>-0.017354544402245</v>
+        <v>-0.01773419684615409</v>
       </c>
     </row>
     <row r="228">
@@ -3393,7 +3393,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>-0.01201748250830957</v>
+        <v>-0.01043800018385233</v>
       </c>
     </row>
     <row r="229">
@@ -3406,7 +3406,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>-0.01749764884435218</v>
+        <v>-0.01452324193252285</v>
       </c>
     </row>
     <row r="230">
@@ -3419,7 +3419,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>-0.02295920696131575</v>
+        <v>-0.02576664637021923</v>
       </c>
     </row>
     <row r="231">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>0.006296701503175798</v>
+        <v>0.007267726416883132</v>
       </c>
     </row>
     <row r="232">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>0.02069699564039521</v>
+        <v>0.02550361192322478</v>
       </c>
     </row>
     <row r="233">
@@ -3458,7 +3458,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>0.01862942893558944</v>
+        <v>0.01907872696845351</v>
       </c>
     </row>
     <row r="234">
@@ -3471,7 +3471,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>-0.005603844661007247</v>
+        <v>-0.008736955934102916</v>
       </c>
     </row>
     <row r="235">
@@ -3484,7 +3484,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0.005870001774826479</v>
+        <v>0.006653458249292948</v>
       </c>
     </row>
     <row r="236">
@@ -3497,7 +3497,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>-0.02728220219856165</v>
+        <v>-0.02813723751154162</v>
       </c>
     </row>
     <row r="237">
@@ -3510,7 +3510,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>0.004494239024913665</v>
+        <v>0.008222755613350003</v>
       </c>
     </row>
     <row r="238">
@@ -3523,7 +3523,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>6.920506286414241e-05</v>
+        <v>-0.0001798456461713563</v>
       </c>
     </row>
     <row r="239">
@@ -3536,7 +3536,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>0.01314995408480837</v>
+        <v>0.008781634369500156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mudanças no valor dos parametros, para teste
</commit_message>
<xml_diff>
--- a/data/results/df_daily_return_ppo.xlsx
+++ b/data/results/df_daily_return_ppo.xlsx
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.02051435734447838</v>
+        <v>0.02137985199563299</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.0001375096831625344</v>
+        <v>-0.002363510765643739</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8.305288303231905e-05</v>
+        <v>0.001179769784898359</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.02579723778711187</v>
+        <v>0.02724196883511882</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.005825733028860881</v>
+        <v>-0.008100894459429865</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.005833829896371486</v>
+        <v>0.00650143196516457</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.001062550162739401</v>
+        <v>0.001858025266165889</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.002332471335930176</v>
+        <v>-0.003321351487738728</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.003576702922601704</v>
+        <v>-0.006452902348468657</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.003106258467134456</v>
+        <v>0.006237167780109235</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01984543428669502</v>
+        <v>0.02232757518816721</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.003023307893114284</v>
+        <v>0.003493251961255815</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.01938765214175742</v>
+        <v>0.01598890342849695</v>
       </c>
     </row>
     <row r="16">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.002660651770497854</v>
+        <v>-0.0005419984210727371</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.002590669954575491</v>
+        <v>0.001476106481723344</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.0234845557800854</v>
+        <v>-0.02070394693157971</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.03509710545456971</v>
+        <v>-0.0368564206679339</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.009562527717395372</v>
+        <v>-0.000293274743787652</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.02349751251101369</v>
+        <v>-0.02120373330387478</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.02162647400210408</v>
+        <v>0.02381799825166052</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.00937492454114998</v>
+        <v>0.0100803352480137</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.01968607346541905</v>
+        <v>0.02359622284872749</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.004563834505195126</v>
+        <v>-0.004745545383775887</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.03273956033000804</v>
+        <v>0.02579647511805331</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.03130790025388665</v>
+        <v>0.02858101005920386</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.006714583845418093</v>
+        <v>-0.007046671725357694</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.02197151076693475</v>
+        <v>-0.02374492999781658</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.02041100812541597</v>
+        <v>0.01868336912167892</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.0168547971460298</v>
+        <v>0.02006694505122338</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.005076559319618838</v>
+        <v>0.000948275695208654</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.01143158872470887</v>
+        <v>-0.01155980422096776</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.000223076087560152</v>
+        <v>0.001351381877059201</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.00304450553521832</v>
+        <v>0.001904908533993321</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.02390376518836063</v>
+        <v>0.02526351118386569</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.003251529956255575</v>
+        <v>-0.002992759592463575</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.003936250235822492</v>
+        <v>0.006444033172806448</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.00562469631379969</v>
+        <v>0.005363363098317457</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>-0.01473252992039143</v>
+        <v>-0.01113563577858526</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.02850867434981026</v>
+        <v>0.0275323484633831</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.006143394398916415</v>
+        <v>-0.0003096459257091158</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>-0.003455378746039343</v>
+        <v>-0.009853486572788546</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.01430316425622114</v>
+        <v>0.0142960478587319</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>-0.001512551533702053</v>
+        <v>-0.0003658115558731228</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.001734896453142683</v>
+        <v>0.004499535636574766</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.002394796986218513</v>
+        <v>0.002922654330576122</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.02596154307477862</v>
+        <v>0.027041231993138</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.01054674349189588</v>
+        <v>0.006751732913931214</v>
       </c>
     </row>
     <row r="50">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>-0.006902313585903123</v>
+        <v>-0.007623223647902435</v>
       </c>
     </row>
     <row r="51">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.01074859235451519</v>
+        <v>0.01066999356698596</v>
       </c>
     </row>
     <row r="52">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.01468183974347432</v>
+        <v>0.01220500996144438</v>
       </c>
     </row>
     <row r="53">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.003302991955857197</v>
+        <v>0.002733294813112483</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.001076453461456259</v>
+        <v>-0.000888992128630597</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>-0.02072208113356628</v>
+        <v>-0.02290802799442766</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.01110123930485388</v>
+        <v>0.008622600657095421</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.003729709518888322</v>
+        <v>0.00191132502124998</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.01062753540114113</v>
+        <v>0.009732875918254117</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.00462609702168591</v>
+        <v>0.003476308580482171</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.000702327383818287</v>
+        <v>0.001579436681926505</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>-0.007064380390388275</v>
+        <v>-0.01236255200467162</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.0007140330785131938</v>
+        <v>0.002147186311845606</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.01036101706502311</v>
+        <v>0.005856230708811629</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.03509093659862879</v>
+        <v>0.03031446829283975</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.01534233037558532</v>
+        <v>0.01189001645332935</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>-0.01707234452328786</v>
+        <v>-0.01698817753223639</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>-0.008482911060907056</v>
+        <v>-0.015464951702032</v>
       </c>
     </row>
     <row r="68">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.007543263013162283</v>
+        <v>0.005833421912258706</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>-0.02119585294863701</v>
+        <v>-0.02221940915290645</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.003720045829255648</v>
+        <v>0.004461539903535414</v>
       </c>
     </row>
     <row r="71">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-0.002297676235293499</v>
+        <v>-0.0018318344683017</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>-0.009945297379298963</v>
+        <v>-0.009296953035759848</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>-0.01154810866095678</v>
+        <v>-0.01257928021165823</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>-0.01311149138160481</v>
+        <v>-0.0105770767804971</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>-0.01042533578900092</v>
+        <v>-0.01125136770389764</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>-0.002715381752200662</v>
+        <v>0.00154035649412227</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.0244933068019604</v>
+        <v>0.02104557409972133</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>-0.02483406411740836</v>
+        <v>-0.02362211492631657</v>
       </c>
     </row>
     <row r="79">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.03319973157667867</v>
+        <v>0.02164006642499902</v>
       </c>
     </row>
     <row r="80">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.002697138856993156</v>
+        <v>-0.001906346635009698</v>
       </c>
     </row>
     <row r="81">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.01400880246388621</v>
+        <v>0.01476753714813669</v>
       </c>
     </row>
     <row r="82">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-0.002874348434137302</v>
+        <v>-0.002668327573790858</v>
       </c>
     </row>
     <row r="83">
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.007324260532039726</v>
+        <v>0.005486248812429724</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>-0.01215943203034563</v>
+        <v>-0.01032206187686118</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>-0.002421900685187426</v>
+        <v>-0.002295142513866082</v>
       </c>
     </row>
     <row r="86">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.003628164412089449</v>
+        <v>-0.001776499887729259</v>
       </c>
     </row>
     <row r="87">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.005691173313013595</v>
+        <v>0.009290627105531983</v>
       </c>
     </row>
     <row r="88">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.00596927349170409</v>
+        <v>-0.002348799020813868</v>
       </c>
     </row>
     <row r="89">
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>-0.008087148964457953</v>
+        <v>-0.007870541145766661</v>
       </c>
     </row>
     <row r="90">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>-0.04012147107749704</v>
+        <v>-0.04073413677139905</v>
       </c>
     </row>
     <row r="91">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.02840371658338257</v>
+        <v>0.03342228641041373</v>
       </c>
     </row>
     <row r="92">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.004112370370237574</v>
+        <v>0.004350963860074735</v>
       </c>
     </row>
     <row r="93">
@@ -1638,7 +1638,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>-0.02763824681084825</v>
+        <v>-0.02730015091936916</v>
       </c>
     </row>
     <row r="94">
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>-0.02607174950369251</v>
+        <v>-0.02403948539903868</v>
       </c>
     </row>
     <row r="95">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>-0.007797282794926744</v>
+        <v>-0.002379776795165678</v>
       </c>
     </row>
     <row r="96">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.01471953368257418</v>
+        <v>0.01461675317629078</v>
       </c>
     </row>
     <row r="97">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>-0.001474980147440118</v>
+        <v>-0.002280764047668402</v>
       </c>
     </row>
     <row r="98">
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.01559001060992371</v>
+        <v>0.01131910893870569</v>
       </c>
     </row>
     <row r="99">
@@ -1716,7 +1716,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.02569882639031697</v>
+        <v>0.02317099838937734</v>
       </c>
     </row>
     <row r="100">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>-0.03091127204215155</v>
+        <v>-0.03633336638682191</v>
       </c>
     </row>
     <row r="101">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.006646597485941096</v>
+        <v>0.01148791115150462</v>
       </c>
     </row>
     <row r="102">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.0005699146127152468</v>
+        <v>0.0007265508313804115</v>
       </c>
     </row>
     <row r="103">
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.006742942533548534</v>
+        <v>0.003401344542036777</v>
       </c>
     </row>
     <row r="104">
@@ -1781,7 +1781,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.001954806305100986</v>
+        <v>0.004944224932907377</v>
       </c>
     </row>
     <row r="105">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>-0.0039505552793445</v>
+        <v>-0.00470689308986458</v>
       </c>
     </row>
     <row r="106">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.02467569038113664</v>
+        <v>0.03057090892785369</v>
       </c>
     </row>
     <row r="107">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>-2.882217516871977e-09</v>
+        <v>-0.003892893855074946</v>
       </c>
     </row>
     <row r="108">
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.006015641209137247</v>
+        <v>0.006942543479512731</v>
       </c>
     </row>
     <row r="109">
@@ -1846,7 +1846,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>-0.006722776516889137</v>
+        <v>-0.007633395293186273</v>
       </c>
     </row>
     <row r="110">
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>-0.01799979337725179</v>
+        <v>-0.01425167141537881</v>
       </c>
     </row>
     <row r="111">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>-0.003963768538029548</v>
+        <v>-0.008859233811102419</v>
       </c>
     </row>
     <row r="112">
@@ -1885,7 +1885,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.008903434169700047</v>
+        <v>0.01146056067765886</v>
       </c>
     </row>
     <row r="113">
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0.005847704722471756</v>
+        <v>0.003263579508641823</v>
       </c>
     </row>
     <row r="114">
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0.003426285765308</v>
+        <v>-0.001044811566480188</v>
       </c>
     </row>
     <row r="115">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0.006332856739910029</v>
+        <v>0.01155934172357759</v>
       </c>
     </row>
     <row r="116">
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>-0.0125420167111633</v>
+        <v>-0.008641660341939281</v>
       </c>
     </row>
     <row r="117">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>-0.01179917410818732</v>
+        <v>-0.0119362031970099</v>
       </c>
     </row>
     <row r="118">
@@ -1963,7 +1963,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.01643064835245211</v>
+        <v>0.01688781697570529</v>
       </c>
     </row>
     <row r="119">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.003525043946617817</v>
+        <v>0.008407271545154697</v>
       </c>
     </row>
     <row r="120">
@@ -1989,7 +1989,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>-0.002078726052475914</v>
+        <v>0.002772538325388135</v>
       </c>
     </row>
     <row r="121">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>0.002164242777852014</v>
+        <v>0.0003409288036864399</v>
       </c>
     </row>
     <row r="122">
@@ -2015,7 +2015,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>-0.002859765380563018</v>
+        <v>-0.002162913220794407</v>
       </c>
     </row>
     <row r="123">
@@ -2028,7 +2028,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0.004322631166222414</v>
+        <v>0.009305452338062421</v>
       </c>
     </row>
     <row r="124">
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.005303860478761781</v>
+        <v>0.00377805338930386</v>
       </c>
     </row>
     <row r="125">
@@ -2054,7 +2054,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>-0.0001956274324654864</v>
+        <v>-0.001901391332240986</v>
       </c>
     </row>
     <row r="126">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.007696609866311753</v>
+        <v>0.005645973118022411</v>
       </c>
     </row>
     <row r="127">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>-0.0007573142225246489</v>
+        <v>0.003827588045141742</v>
       </c>
     </row>
     <row r="128">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>-0.001560109965805489</v>
+        <v>-0.002807321700784905</v>
       </c>
     </row>
     <row r="129">
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>-0.01022275002372063</v>
+        <v>-0.006965220850574428</v>
       </c>
     </row>
     <row r="130">
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.008583934823638575</v>
+        <v>0.01055117159050621</v>
       </c>
     </row>
     <row r="131">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>-0.0001824346804232672</v>
+        <v>-0.001747525334170657</v>
       </c>
     </row>
     <row r="132">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>-0.008253877124021522</v>
+        <v>-0.006157825853235213</v>
       </c>
     </row>
     <row r="133">
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.01370940638795208</v>
+        <v>0.01341405575008687</v>
       </c>
     </row>
     <row r="134">
@@ -2171,7 +2171,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>-0.01087496546452281</v>
+        <v>-0.009330366542548362</v>
       </c>
     </row>
     <row r="135">
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>-0.00670681117881388</v>
+        <v>-0.006312539860502399</v>
       </c>
     </row>
     <row r="136">
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0.0003534827281194825</v>
+        <v>0.003690189527614077</v>
       </c>
     </row>
     <row r="137">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>-0.01561519106763043</v>
+        <v>-0.01147747539518361</v>
       </c>
     </row>
     <row r="138">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0.01238964605658738</v>
+        <v>0.01622229683506747</v>
       </c>
     </row>
     <row r="139">
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.01744952423345932</v>
+        <v>0.005391884584509696</v>
       </c>
     </row>
     <row r="140">
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.01752793642547214</v>
+        <v>0.0182029909238456</v>
       </c>
     </row>
     <row r="141">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.006835324500154278</v>
+        <v>0.003894819767174509</v>
       </c>
     </row>
     <row r="142">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.01278594182128768</v>
+        <v>0.01339264215423673</v>
       </c>
     </row>
     <row r="143">
@@ -2288,7 +2288,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>-0.01427568334127211</v>
+        <v>-0.009187898933436233</v>
       </c>
     </row>
     <row r="144">
@@ -2301,7 +2301,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0.003651490887585052</v>
+        <v>0.005319966672649304</v>
       </c>
     </row>
     <row r="145">
@@ -2314,7 +2314,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>0.005677704740940499</v>
+        <v>0.007482301306704307</v>
       </c>
     </row>
     <row r="146">
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>-0.003000005836666262</v>
+        <v>-0.002450390724302177</v>
       </c>
     </row>
     <row r="147">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0.004065849617040903</v>
+        <v>0.003187512803056511</v>
       </c>
     </row>
     <row r="148">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>-0.006375744118700048</v>
+        <v>-0.003956214682095633</v>
       </c>
     </row>
     <row r="149">
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0.002622863141209583</v>
+        <v>0.001136991948692946</v>
       </c>
     </row>
     <row r="150">
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0.004908013828907936</v>
+        <v>0.005298506255925592</v>
       </c>
     </row>
     <row r="151">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>-0.004629905320527777</v>
+        <v>-0.00567397668309172</v>
       </c>
     </row>
     <row r="152">
@@ -2405,7 +2405,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.0006404891491440541</v>
+        <v>0.001795343774043694</v>
       </c>
     </row>
     <row r="153">
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0.007967088109164751</v>
+        <v>0.004748170386877056</v>
       </c>
     </row>
     <row r="154">
@@ -2431,7 +2431,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0.01181414693332584</v>
+        <v>0.007687357465344762</v>
       </c>
     </row>
     <row r="155">
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.003825242124547813</v>
+        <v>0.002287710239272339</v>
       </c>
     </row>
     <row r="156">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.01011541755906155</v>
+        <v>0.01314652901365308</v>
       </c>
     </row>
     <row r="157">
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0.01365382847329401</v>
+        <v>0.00796988314842443</v>
       </c>
     </row>
     <row r="158">
@@ -2483,7 +2483,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0.003012637547863795</v>
+        <v>0.005380565152859334</v>
       </c>
     </row>
     <row r="159">
@@ -2496,7 +2496,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0.009378398246148414</v>
+        <v>0.009313024933842467</v>
       </c>
     </row>
     <row r="160">
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>-0.01247314440124957</v>
+        <v>-0.009919914780157781</v>
       </c>
     </row>
     <row r="161">
@@ -2522,7 +2522,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.00653557361899672</v>
+        <v>0.003298722790361665</v>
       </c>
     </row>
     <row r="162">
@@ -2535,7 +2535,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>-0.003006329698577769</v>
+        <v>-0.00346418906684668</v>
       </c>
     </row>
     <row r="163">
@@ -2548,7 +2548,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>-0.003435693108366187</v>
+        <v>-0.002929440986087843</v>
       </c>
     </row>
     <row r="164">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.001852228325471234</v>
+        <v>0.00219147531696155</v>
       </c>
     </row>
     <row r="165">
@@ -2574,7 +2574,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>-0.00162286970867853</v>
+        <v>-5.875332786330252e-06</v>
       </c>
     </row>
     <row r="166">
@@ -2587,7 +2587,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0.002493088547234747</v>
+        <v>0.000402702267033334</v>
       </c>
     </row>
     <row r="167">
@@ -2600,7 +2600,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-0.009718040162592183</v>
+        <v>-0.01392132533215111</v>
       </c>
     </row>
     <row r="168">
@@ -2613,7 +2613,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0.005030412385775558</v>
+        <v>0.009765122833374712</v>
       </c>
     </row>
     <row r="169">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0.004407655294694672</v>
+        <v>0.005697236952594147</v>
       </c>
     </row>
     <row r="170">
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-0.0056761141820567</v>
+        <v>-0.008858988309709125</v>
       </c>
     </row>
     <row r="171">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-0.006064460760590201</v>
+        <v>-0.00513639954444624</v>
       </c>
     </row>
     <row r="172">
@@ -2665,7 +2665,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.005978634671996524</v>
+        <v>0.003565329674412763</v>
       </c>
     </row>
     <row r="173">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-0.02571027288664712</v>
+        <v>-0.02405530953019877</v>
       </c>
     </row>
     <row r="174">
@@ -2691,7 +2691,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.007106320428541879</v>
+        <v>0.007608696616885252</v>
       </c>
     </row>
     <row r="175">
@@ -2704,7 +2704,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-0.002320187228931714</v>
+        <v>-0.00341334476004958</v>
       </c>
     </row>
     <row r="176">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-0.006900590831603003</v>
+        <v>-0.007653449613313143</v>
       </c>
     </row>
     <row r="177">
@@ -2730,7 +2730,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-0.004480738624410435</v>
+        <v>-0.004598374863028805</v>
       </c>
     </row>
     <row r="178">
@@ -2743,7 +2743,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0.007178835180708563</v>
+        <v>0.007219211333272089</v>
       </c>
     </row>
     <row r="179">
@@ -2756,7 +2756,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-0.007185451704328711</v>
+        <v>-0.002472506716541562</v>
       </c>
     </row>
     <row r="180">
@@ -2769,7 +2769,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-0.01316678247773962</v>
+        <v>-0.01318517061027527</v>
       </c>
     </row>
     <row r="181">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0.01240361774214449</v>
+        <v>0.01443224988452969</v>
       </c>
     </row>
     <row r="182">
@@ -2795,7 +2795,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-0.01498133765061826</v>
+        <v>-0.0139223821418952</v>
       </c>
     </row>
     <row r="183">
@@ -2808,7 +2808,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0.02140856308580248</v>
+        <v>0.01365919127300252</v>
       </c>
     </row>
     <row r="184">
@@ -2821,7 +2821,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.001694308919124908</v>
+        <v>0.0006853058252656075</v>
       </c>
     </row>
     <row r="185">
@@ -2834,7 +2834,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-0.01514691091542449</v>
+        <v>-0.01297994026253423</v>
       </c>
     </row>
     <row r="186">
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-0.01292098258228662</v>
+        <v>-0.01121039866977012</v>
       </c>
     </row>
     <row r="187">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-0.01496097660195592</v>
+        <v>-0.01268778775241154</v>
       </c>
     </row>
     <row r="188">
@@ -2873,7 +2873,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.009342703823630286</v>
+        <v>0.009749072170322424</v>
       </c>
     </row>
     <row r="189">
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.002548247118438769</v>
+        <v>0.003792163319445231</v>
       </c>
     </row>
     <row r="190">
@@ -2899,7 +2899,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-0.002894834490577225</v>
+        <v>-0.003594477502607168</v>
       </c>
     </row>
     <row r="191">
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-0.007638100821650799</v>
+        <v>-0.007902744261793153</v>
       </c>
     </row>
     <row r="192">
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0.01176889138947857</v>
+        <v>0.01142652558795412</v>
       </c>
     </row>
     <row r="193">
@@ -2938,7 +2938,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-0.007186315420856699</v>
+        <v>-0.008324232893152329</v>
       </c>
     </row>
     <row r="194">
@@ -2951,7 +2951,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0.01288280046012008</v>
+        <v>0.01488459450221888</v>
       </c>
     </row>
     <row r="195">
@@ -2964,7 +2964,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-0.005986875313075053</v>
+        <v>-0.007069003112487262</v>
       </c>
     </row>
     <row r="196">
@@ -2977,7 +2977,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-0.02953262219820569</v>
+        <v>-0.02933990911844923</v>
       </c>
     </row>
     <row r="197">
@@ -2990,7 +2990,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0.004069016850059181</v>
+        <v>0.006369981418356287</v>
       </c>
     </row>
     <row r="198">
@@ -3003,7 +3003,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.01082593032328428</v>
+        <v>0.009817178147181256</v>
       </c>
     </row>
     <row r="199">
@@ -3016,7 +3016,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-0.01376939399164872</v>
+        <v>-0.01592529058503198</v>
       </c>
     </row>
     <row r="200">
@@ -3029,7 +3029,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-0.006151339332553268</v>
+        <v>0.003271865567805655</v>
       </c>
     </row>
     <row r="201">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0.01452562201090075</v>
+        <v>0.01255585797597131</v>
       </c>
     </row>
     <row r="202">
@@ -3055,7 +3055,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0.004902303994855401</v>
+        <v>0.005173562973077707</v>
       </c>
     </row>
     <row r="203">
@@ -3068,7 +3068,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-0.01234429926445696</v>
+        <v>-0.01173477818611462</v>
       </c>
     </row>
     <row r="204">
@@ -3081,7 +3081,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-0.0042882937356993</v>
+        <v>-0.003586044403051866</v>
       </c>
     </row>
     <row r="205">
@@ -3094,7 +3094,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>0.00033787893669382</v>
+        <v>0.002880541154048066</v>
       </c>
     </row>
     <row r="206">
@@ -3107,7 +3107,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-0.01235769970659253</v>
+        <v>-0.0129410433062244</v>
       </c>
     </row>
     <row r="207">
@@ -3120,7 +3120,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-0.005493907563614209</v>
+        <v>-0.005017105222408229</v>
       </c>
     </row>
     <row r="208">
@@ -3133,7 +3133,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-0.01470581312505657</v>
+        <v>-0.01125185914421897</v>
       </c>
     </row>
     <row r="209">
@@ -3146,7 +3146,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.007271154461730368</v>
+        <v>0.002098335358252166</v>
       </c>
     </row>
     <row r="210">
@@ -3159,7 +3159,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.01335994738926758</v>
+        <v>0.009287665689493104</v>
       </c>
     </row>
     <row r="211">
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-0.005376969424788742</v>
+        <v>-0.00203660317180041</v>
       </c>
     </row>
     <row r="212">
@@ -3185,7 +3185,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>0.02217491077780689</v>
+        <v>0.02172586424763181</v>
       </c>
     </row>
     <row r="213">
@@ -3198,7 +3198,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>0.01018052397502896</v>
+        <v>0.005575909102681398</v>
       </c>
     </row>
     <row r="214">
@@ -3211,7 +3211,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-0.01623462358525367</v>
+        <v>-0.01633733855391164</v>
       </c>
     </row>
     <row r="215">
@@ -3224,7 +3224,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>0.01295285609619496</v>
+        <v>0.01340411236018539</v>
       </c>
     </row>
     <row r="216">
@@ -3237,7 +3237,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-0.006047928473536031</v>
+        <v>-0.005330982918994347</v>
       </c>
     </row>
     <row r="217">
@@ -3250,7 +3250,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>-0.005525642887297968</v>
+        <v>-0.003272512739816044</v>
       </c>
     </row>
     <row r="218">
@@ -3263,7 +3263,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.002625363006218896</v>
+        <v>-0.0002409188314307694</v>
       </c>
     </row>
     <row r="219">
@@ -3276,7 +3276,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>-0.02835702969737758</v>
+        <v>-0.03070188146671999</v>
       </c>
     </row>
     <row r="220">
@@ -3289,7 +3289,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0.001021872997220459</v>
+        <v>0.0001607872331101918</v>
       </c>
     </row>
     <row r="221">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>0.01225389782688378</v>
+        <v>0.01040177622416981</v>
       </c>
     </row>
     <row r="222">
@@ -3315,7 +3315,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>-0.04577073285731705</v>
+        <v>-0.04917669193738473</v>
       </c>
     </row>
     <row r="223">
@@ -3328,7 +3328,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>0.02066984771095196</v>
+        <v>0.02424822406874634</v>
       </c>
     </row>
     <row r="224">
@@ -3341,7 +3341,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>-0.009540201683117264</v>
+        <v>-0.007893618388091141</v>
       </c>
     </row>
     <row r="225">
@@ -3354,7 +3354,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>0.01828071343772742</v>
+        <v>0.01761403410259151</v>
       </c>
     </row>
     <row r="226">
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>-0.0005503458119990293</v>
+        <v>-0.0003401592047834534</v>
       </c>
     </row>
     <row r="227">
@@ -3380,7 +3380,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>-0.01773419684615409</v>
+        <v>-0.01468146104984718</v>
       </c>
     </row>
     <row r="228">
@@ -3393,7 +3393,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>-0.01043800018385233</v>
+        <v>-0.01327940511195662</v>
       </c>
     </row>
     <row r="229">
@@ -3406,7 +3406,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>-0.01452324193252285</v>
+        <v>-0.02027081958039314</v>
       </c>
     </row>
     <row r="230">
@@ -3419,7 +3419,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>-0.02576664637021923</v>
+        <v>-0.02321089723235157</v>
       </c>
     </row>
     <row r="231">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>0.007267726416883132</v>
+        <v>0.006962296852035992</v>
       </c>
     </row>
     <row r="232">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>0.02550361192322478</v>
+        <v>0.02569390679781122</v>
       </c>
     </row>
     <row r="233">
@@ -3458,7 +3458,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>0.01907872696845351</v>
+        <v>0.01697419532839787</v>
       </c>
     </row>
     <row r="234">
@@ -3471,7 +3471,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>-0.008736955934102916</v>
+        <v>-0.008477080071046892</v>
       </c>
     </row>
     <row r="235">
@@ -3484,7 +3484,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0.006653458249292948</v>
+        <v>0.003368824600435838</v>
       </c>
     </row>
     <row r="236">
@@ -3497,7 +3497,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>-0.02813723751154162</v>
+        <v>-0.02535401653662717</v>
       </c>
     </row>
     <row r="237">
@@ -3510,7 +3510,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>0.008222755613350003</v>
+        <v>0.005910691081153945</v>
       </c>
     </row>
     <row r="238">
@@ -3523,7 +3523,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>-0.0001798456461713563</v>
+        <v>0.00119098338597963</v>
       </c>
     </row>
     <row r="239">
@@ -3536,7 +3536,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>0.008781634369500156</v>
+        <v>0.007657126672446532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>